<commit_message>
Nuevo SK_Punto Venta Completo
</commit_message>
<xml_diff>
--- a/Scripts_R110_Catalogos/LIQ19_R110_01.b_CI_Punto_Venta_20190131_JAR.XLSX
+++ b/Scripts_R110_Catalogos/LIQ19_R110_01.b_CI_Punto_Venta_20190131_JAR.XLSX
@@ -471,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -501,6 +501,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -785,10 +786,10 @@
   <dimension ref="B2:R51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomRight" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1038,14 +1039,14 @@
         <v>1</v>
       </c>
       <c r="H9" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9" s="14">
         <v>1</v>
       </c>
       <c r="J9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 8, 'BE01', 'BE0','', 7, 1, 3, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 8, 'BE01', 'BE0','', 7, 1, 2, 1; </v>
       </c>
       <c r="N9" s="1"/>
       <c r="R9" s="3"/>
@@ -1068,14 +1069,14 @@
         <v>1</v>
       </c>
       <c r="H10" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10" s="14">
         <v>1</v>
       </c>
       <c r="J10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 9, 'BE02', 'BE0','', 8, 1, 2, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 9, 'BE02', 'BE0','', 8, 1, 3, 1; </v>
       </c>
       <c r="N10" s="1"/>
       <c r="R10" s="3"/>
@@ -1098,14 +1099,14 @@
         <v>1</v>
       </c>
       <c r="H11" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I11" s="14">
         <v>1</v>
       </c>
       <c r="J11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 11, 'BE05', 'BE0','', 9, 1, 3, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 11, 'BE05', 'BE0','', 9, 1, 1, 1; </v>
       </c>
       <c r="O11" s="7"/>
     </row>
@@ -1160,14 +1161,14 @@
         <v>0</v>
       </c>
       <c r="H13" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>117</v>
       </c>
       <c r="J13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 13, 'BG05', 'BG0','', 11, 0, 1, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 13, 'BG05', 'BG0','', 11, 0, 2, 1; </v>
       </c>
       <c r="O13" s="7"/>
     </row>
@@ -1218,14 +1219,14 @@
         <v>1</v>
       </c>
       <c r="H15" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>117</v>
       </c>
       <c r="J15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 15, 'BG08', 'BG0','', 13, 1, 2, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 15, 'BG08', 'BG0','', 13, 1, 3, 1; </v>
       </c>
       <c r="O15" s="7"/>
     </row>
@@ -1305,14 +1306,14 @@
         <v>1</v>
       </c>
       <c r="H18" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>119</v>
       </c>
       <c r="J18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 18, 'BG11', 'BG1','', 16, 1, 3, 3; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 18, 'BG11', 'BG1','', 16, 1, 2, 3; </v>
       </c>
       <c r="O18" s="8"/>
     </row>
@@ -1363,14 +1364,14 @@
         <v>1</v>
       </c>
       <c r="H20" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I20" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 20, 'BG12', 'BG1','', 18, 1, 2, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 20, 'BG12', 'BG1','', 18, 1, 3, 1; </v>
       </c>
       <c r="O20" s="8"/>
     </row>
@@ -1392,14 +1393,14 @@
         <v>1</v>
       </c>
       <c r="H21" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 21, 'BG19', 'BG1','', 19, 1, 3, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 21, 'BG19', 'BG1','', 19, 1, 1, 1; </v>
       </c>
       <c r="O21" s="8"/>
     </row>
@@ -1450,14 +1451,14 @@
         <v>0</v>
       </c>
       <c r="H23" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 23, 'BG21', 'BG2','', 21, 0, 1, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 23, 'BG21', 'BG2','', 21, 0, 2, 1; </v>
       </c>
       <c r="O23" s="8"/>
     </row>
@@ -1478,7 +1479,7 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="17">
         <v>3</v>
       </c>
       <c r="I24" s="13" t="s">
@@ -1508,14 +1509,14 @@
         <v>1</v>
       </c>
       <c r="H25" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I25" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 25, 'BG27', 'BG2','', 23, 1, 2, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 25, 'BG27', 'BG2','', 23, 1, 3, 1; </v>
       </c>
       <c r="O25" s="8"/>
     </row>
@@ -1595,14 +1596,14 @@
         <v>1</v>
       </c>
       <c r="H28" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 28, 'BG31', 'BG3','', 26, 1, 3, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 28, 'BG31', 'BG3','', 26, 1, 2, 1; </v>
       </c>
       <c r="O28" s="8"/>
     </row>
@@ -1653,14 +1654,14 @@
         <v>1</v>
       </c>
       <c r="H30" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 30, 'U55 EXP', 'U55','', 28, 1, 2, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 30, 'U55 EXP', 'U55','', 28, 1, 3, 1; </v>
       </c>
       <c r="O30" s="8"/>
     </row>
@@ -1682,14 +1683,14 @@
         <v>1</v>
       </c>
       <c r="H31" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J31" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 31, 'C121', 'C12','', 29, 1, 3, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 31, 'C121', 'C12','', 29, 1, 1, 1; </v>
       </c>
       <c r="O31" s="8"/>
     </row>
@@ -1740,14 +1741,14 @@
         <v>0</v>
       </c>
       <c r="H33" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I33" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J33" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 33, 'C134', 'C13','', 31, 0, 1, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 33, 'C134', 'C13','', 31, 0, 3, 1; </v>
       </c>
       <c r="O33" s="8"/>
     </row>
@@ -1769,14 +1770,14 @@
         <v>1</v>
       </c>
       <c r="H34" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34" s="13" t="s">
         <v>118</v>
       </c>
       <c r="J34" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 34, 'C122', 'C12','', 32, 1, 3, 2; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 34, 'C122', 'C12','', 32, 1, 2, 2; </v>
       </c>
       <c r="O34" s="8"/>
     </row>
@@ -1798,14 +1799,14 @@
         <v>1</v>
       </c>
       <c r="H35" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I35" s="13" t="s">
         <v>118</v>
       </c>
       <c r="J35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 35, 'C123', 'C12','', 33, 1, 2, 2; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 35, 'C123', 'C12','', 33, 1, 3, 2; </v>
       </c>
       <c r="O35" s="8"/>
     </row>
@@ -1885,14 +1886,14 @@
         <v>1</v>
       </c>
       <c r="H38" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>118</v>
       </c>
       <c r="J38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 38, 'C126', 'C12','', 36, 1, 3, 2; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 38, 'C126', 'C12','', 36, 1, 2, 2; </v>
       </c>
       <c r="O38" s="8"/>
     </row>
@@ -1943,14 +1944,14 @@
         <v>1</v>
       </c>
       <c r="H40" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I40" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 40, 'C128', 'C12','', 38, 1, 2, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 40, 'C128', 'C12','', 38, 1, 3, 1; </v>
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.45">
@@ -1971,14 +1972,14 @@
         <v>1</v>
       </c>
       <c r="H41" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I41" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 41, 'C129', 'C12','', 39, 1, 3, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 41, 'C129', 'C12','', 39, 1, 1, 1; </v>
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.45">
@@ -2027,14 +2028,14 @@
         <v>0</v>
       </c>
       <c r="H43" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 43, 'C131', 'C13','', 41, 0, 1, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 43, 'C131', 'C13','', 41, 0, 2, 1; </v>
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.45">
@@ -2083,14 +2084,14 @@
         <v>1</v>
       </c>
       <c r="H45" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I45" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 45, 'C02', 'C02','', 43, 1, 2, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 45, 'C02', 'C02','', 43, 1, 3, 1; </v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.45">
@@ -2167,14 +2168,14 @@
         <v>1</v>
       </c>
       <c r="H48" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I48" s="13" t="s">
         <v>117</v>
       </c>
       <c r="J48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 48, 'U02', 'U02','', 46, 1, 3, 1; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 48, 'U02', 'U02','', 46, 1, 2, 1; </v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.45">
@@ -2195,14 +2196,14 @@
         <v>1</v>
       </c>
       <c r="H49" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I49" s="13" t="s">
         <v>118</v>
       </c>
       <c r="J49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 49, 'U46', 'U46','', 47, 1, 3, 2; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_PUNTO_VENTA] 0,0, 49, 'U46', 'U46','', 47, 1, 2, 2; </v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.45">

</xml_diff>